<commit_message>
Update historical Russia coding
</commit_message>
<xml_diff>
--- a/BastianHerre/biological_chemical_weapons/OWID based on Arms Control Association (2022), Nuclear Threat Initiative (2022), Center for Nonproliferation Studies (2008), and UN (2022) biological and chemical weapons proliferation/biological_chemical_weapons_proliferation_raw.xlsx
+++ b/BastianHerre/biological_chemical_weapons/OWID based on Arms Control Association (2022), Nuclear Threat Initiative (2022), Center for Nonproliferation Studies (2008), and UN (2022) biological and chemical weapons proliferation/biological_chemical_weapons_proliferation_raw.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bastianherre/Dropbox/Data/biological_chemical_weapons/OWID based on Arms Control Association (2022), Nuclear Threat Initiative (2022), Center for Nonproliferation Studies (2008), and UN (2022) biological and chemical weapons proliferation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40145B9-FE90-ED4C-BD13-2F55D1FC6B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BF0FA3-A37F-1940-8DBB-26C575474702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7850FBFA-5780-AC4A-BE88-30DAFDB7324F}"/>
   </bookViews>
@@ -1073,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58AD4FA3-34FF-4344-90DC-F9D510392035}">
   <dimension ref="A1:H198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="G147" sqref="G147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4904,7 +4904,7 @@
         <v>209</v>
       </c>
       <c r="G147" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="H147" t="s">
         <v>204</v>

</xml_diff>

<commit_message>
Update Austria, Germany, Italy, and Spain coding
</commit_message>
<xml_diff>
--- a/BastianHerre/biological_chemical_weapons/OWID based on Arms Control Association (2022), Nuclear Threat Initiative (2022), Center for Nonproliferation Studies (2008), and UN (2022) biological and chemical weapons proliferation/biological_chemical_weapons_proliferation_raw.xlsx
+++ b/BastianHerre/biological_chemical_weapons/OWID based on Arms Control Association (2022), Nuclear Threat Initiative (2022), Center for Nonproliferation Studies (2008), and UN (2022) biological and chemical weapons proliferation/biological_chemical_weapons_proliferation_raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bastianherre/Dropbox/Data/biological_chemical_weapons/OWID based on Arms Control Association (2022), Nuclear Threat Initiative (2022), Center for Nonproliferation Studies (2008), and UN (2022) biological and chemical weapons proliferation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BF0FA3-A37F-1940-8DBB-26C575474702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB95F1B4-3BCF-0141-9B70-3872CE548089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7850FBFA-5780-AC4A-BE88-30DAFDB7324F}"/>
   </bookViews>
@@ -1073,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58AD4FA3-34FF-4344-90DC-F9D510392035}">
   <dimension ref="A1:H198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="G147" sqref="G147"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="G168" sqref="G168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1368,7 +1368,7 @@
         <v>212</v>
       </c>
       <c r="G11" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="H11" t="s">
         <v>204</v>
@@ -2824,7 +2824,7 @@
         <v>212</v>
       </c>
       <c r="G67" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H67" t="s">
         <v>204</v>
@@ -3318,7 +3318,7 @@
         <v>212</v>
       </c>
       <c r="G86" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H86" t="s">
         <v>204</v>
@@ -5450,7 +5450,7 @@
         <v>212</v>
       </c>
       <c r="G168" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="H168" t="s">
         <v>204</v>

</xml_diff>